<commit_message>
Setting up new branch for development of optical material integration in PAOS
</commit_message>
<xml_diff>
--- a/lens data/PAOS_TEL_COM_FGS1_v01.xlsx
+++ b/lens data/PAOS_TEL_COM_FGS1_v01.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="61">
   <si>
     <t xml:space="preserve">INIT</t>
   </si>
@@ -166,13 +166,28 @@
     <t xml:space="preserve">FGS_M1</t>
   </si>
   <si>
-    <t xml:space="preserve">FGS_M2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paraxial Lens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FGS_L</t>
+    <t xml:space="preserve">FGS M2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FGS D3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BK7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FGS D4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPACE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move to LS1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FGS LS1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move to FP</t>
   </si>
   <si>
     <t xml:space="preserve">IMAGE_PLANE</t>
@@ -282,7 +297,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -292,6 +307,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -319,16 +338,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1200,16 +1223,15 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="2" style="0" width="12.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1272,16 +1294,13 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.89"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1321,27 +1340,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E4" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J21" activeCellId="0" sqref="J21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="3" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="12.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="6.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="5.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="5.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="4" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="13.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="10.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="14.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="19" style="0" width="12.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1401,651 +1419,747 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="n">
+      <c r="A2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="4" t="n">
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="5" t="n">
         <v>0.55</v>
       </c>
-      <c r="K2" s="4" t="n">
+      <c r="K2" s="5" t="n">
         <v>0.55</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="n">
+      <c r="A3" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4" t="n">
+      <c r="G3" s="7"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5" t="n">
         <v>0.1</v>
       </c>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="n">
+      <c r="A4" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="6"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4" t="n">
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="5" t="n">
         <v>-0.5</v>
       </c>
-      <c r="N4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="n">
+      <c r="A5" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4" t="n">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4" t="s">
+      <c r="E5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="6" t="n">
+      <c r="G5" s="7" t="n">
         <v>-2.319432</v>
       </c>
-      <c r="H5" s="6" t="n">
+      <c r="H5" s="7" t="n">
         <v>-1.05</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="4" t="n">
+      <c r="J5" s="5" t="n">
         <v>0.55</v>
       </c>
-      <c r="K5" s="4" t="n">
+      <c r="K5" s="5" t="n">
         <v>0.365</v>
       </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4" t="n">
+      <c r="L5" s="6"/>
+      <c r="M5" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="n">
+      <c r="A6" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="6" t="n">
+      <c r="G6" s="7" t="n">
         <v>-0.239141</v>
       </c>
-      <c r="H6" s="6" t="n">
+      <c r="H6" s="7" t="n">
         <v>1.331249</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="4" t="n">
+      <c r="J6" s="5" t="n">
         <v>0.055</v>
       </c>
-      <c r="K6" s="4" t="n">
+      <c r="K6" s="5" t="n">
         <v>0.04</v>
       </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4" t="n">
+      <c r="L6" s="6"/>
+      <c r="M6" s="5" t="n">
         <v>0.05</v>
       </c>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="n">
+      <c r="A7" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="6" t="n">
+      <c r="H7" s="7" t="n">
         <f aca="false">-G8/2</f>
         <v>0.2548485</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="4" t="n">
+      <c r="I7" s="8"/>
+      <c r="J7" s="5" t="n">
         <v>0.0125</v>
       </c>
-      <c r="K7" s="4" t="n">
+      <c r="K7" s="5" t="n">
         <v>0.0125</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4" t="n">
+      <c r="L7" s="6"/>
+      <c r="M7" s="5" t="n">
         <v>0.025</v>
       </c>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="n">
+      <c r="A8" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4" t="s">
+      <c r="C8" s="6"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="6" t="n">
+      <c r="G8" s="7" t="n">
         <v>-0.509697</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="7" t="s">
+      <c r="H8" s="7"/>
+      <c r="I8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="4" t="n">
+      <c r="J8" s="5" t="n">
         <v>0.014</v>
       </c>
-      <c r="K8" s="4" t="n">
+      <c r="K8" s="5" t="n">
         <v>0.01</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4" t="n">
+      <c r="L8" s="5"/>
+      <c r="M8" s="5" t="n">
         <v>0.02</v>
       </c>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
+      <c r="N8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="n">
+      <c r="A9" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="6"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4" t="s">
+      <c r="E9" s="5"/>
+      <c r="F9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4" t="n">
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5" t="n">
         <v>0.019873</v>
       </c>
-      <c r="N9" s="4" t="n">
+      <c r="N9" s="5" t="n">
         <v>-5.508</v>
       </c>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="n">
+      <c r="A10" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4" t="s">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="H10" s="6" t="n">
+      <c r="H10" s="7" t="n">
         <v>-0.201646</v>
       </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="n">
+      <c r="A11" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4" t="s">
+      <c r="C11" s="6"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4" t="n">
+      <c r="G11" s="7"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5" t="n">
         <v>-48.329</v>
       </c>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="n">
+      <c r="A12" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4" t="s">
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="7" t="s">
+      <c r="H12" s="7"/>
+      <c r="I12" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="J12" s="4" t="n">
+      <c r="J12" s="5" t="n">
         <v>0.012</v>
       </c>
-      <c r="K12" s="4" t="n">
+      <c r="K12" s="5" t="n">
         <f aca="false">J12</f>
         <v>0.012</v>
       </c>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="n">
+      <c r="A13" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4" t="s">
+      <c r="C13" s="6"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6" t="n">
+      <c r="G13" s="7"/>
+      <c r="H13" s="7" t="n">
         <v>0.1</v>
       </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="8" t="n">
+      <c r="I13" s="7"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="9" t="n">
         <f aca="false">N11</f>
         <v>-48.329</v>
       </c>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="n">
+      <c r="O13" s="5"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5" t="s">
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="9" t="n">
+      <c r="H14" s="11" t="n">
         <f aca="false">0.448168+0.248982+0.009959+0.494036+0.096</f>
         <v>1.297145</v>
       </c>
-      <c r="I14" s="7"/>
-      <c r="J14" s="4" t="n">
+      <c r="I14" s="8"/>
+      <c r="J14" s="5" t="n">
         <v>0.02</v>
       </c>
-      <c r="K14" s="4" t="n">
+      <c r="K14" s="5" t="n">
         <v>0.0067</v>
       </c>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="n">
+      <c r="L14" s="6"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="5" t="n">
+      <c r="C15" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D15" s="6"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5" t="s">
+      <c r="E15" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="4" t="n">
+      <c r="G15" s="7"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="5" t="n">
         <v>0.02</v>
       </c>
-      <c r="K15" s="4" t="n">
+      <c r="K15" s="5" t="n">
         <v>0.0067</v>
       </c>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
-      <c r="N15" s="4"/>
-      <c r="P15" s="4" t="s">
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="n">
+      <c r="A16" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5" t="s">
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G16" s="7" t="n">
-        <v>0.134015</v>
-      </c>
-      <c r="H16" s="9" t="n">
-        <v>0.066999</v>
-      </c>
-      <c r="I16" s="7" t="s">
+      <c r="G16" s="8" t="n">
+        <v>-0.134015</v>
+      </c>
+      <c r="H16" s="11" t="n">
+        <f aca="false">-0.066999</f>
+        <v>-0.066999</v>
+      </c>
+      <c r="I16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="J16" s="4" t="n">
+      <c r="J16" s="5" t="n">
         <v>0.015</v>
       </c>
-      <c r="K16" s="4" t="n">
+      <c r="K16" s="5" t="n">
         <v>0.015</v>
       </c>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="n">
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="5"/>
+      <c r="C17" s="6"/>
       <c r="D17" s="6"/>
-      <c r="E17" s="5" t="n">
+      <c r="E17" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H17" s="6" t="n">
-        <v>0.019653</v>
-      </c>
-      <c r="I17" s="6"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
+      <c r="H17" s="7" t="n">
+        <v>-0.019653</v>
+      </c>
+      <c r="I17" s="7"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="n">
+      <c r="A18" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5" t="n">
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="G18" s="6" t="n">
-        <v>-0.034647</v>
-      </c>
-      <c r="H18" s="9" t="n">
-        <f aca="false">(0.07978+0.0107+0.002+0.004+0.0058+0.002)</f>
-        <v>0.10428</v>
-      </c>
-      <c r="I18" s="6" t="s">
+      <c r="G18" s="7" t="n">
+        <v>0.034647</v>
+      </c>
+      <c r="H18" s="11" t="n">
+        <v>0.07978</v>
+      </c>
+      <c r="I18" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="J18" s="5" t="n">
+      <c r="J18" s="6" t="n">
         <v>0.005</v>
       </c>
-      <c r="K18" s="5" t="n">
+      <c r="K18" s="6" t="n">
         <v>0.005</v>
       </c>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="n">
+      <c r="A19" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" s="5" t="s">
+      <c r="G19" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="8" t="n">
+        <v>0.0107</v>
+      </c>
+      <c r="I19" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G19" s="11" t="n">
-        <v>0.030712</v>
-      </c>
-      <c r="H19" s="9" t="n">
-        <f aca="false">0.003+0.032003</f>
-        <v>0.035003</v>
-      </c>
-      <c r="I19" s="6"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="n">
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4" t="n">
+      <c r="E20" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="6" t="s">
         <v>50</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
+      <c r="H20" s="8" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" s="8" t="n">
+        <f aca="false">0.004+0.0058+0.002</f>
+        <v>0.0118</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="13" t="n">
+        <v>-0.085</v>
+      </c>
+      <c r="H22" s="11" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23" s="11" t="n">
+        <v>0.030721</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G1:G4 I1:P1 I9:I11 G9 G11 I3:L4 I2 L2:P2 N5:P8 P3:P4 N10:P10 P9 N12:P12 P11 P13 N14:P16 L7:M16 I19:P1048576 G20:G1048576 G18 I18:I1048576 J17:P18 G13:G17 I16:I17 J7:K13 J16:K16 I13 I14:K15">
+  <conditionalFormatting sqref="L16:P1048576 L1:P2 G1:G4 I1:I4 I9:K11 J7:K8 J1:K1 J3:K4 G9 G11 I23:I1048576 J12:K1048576 I13:I19 G13:G1048576 L3:L14 O4:P14 M7:M14 O3:P3 N4:N8 N14 N10 N12 L15:O1048576 P15">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>$B1 = "Prism"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D4 G1:I4 L1:O2 G9:I9 G11:I11 I10 H12 I13 L3:L4 N5:O8 N10:O10 N12:O12 N14:O16 L7:M16 H14:I1048576 D18:D1048576 G20:G1048576 G18 Q18:R1048576 L17:O1048576 D6:D17 G13:G17 Q1:R17">
+  <conditionalFormatting sqref="Q10:R1048576 D10:D1048576 I23:I1048576 L1:O2 Q1:R9 D1:D9 G1:I4 G9:H9 G25:H1048576 I9:I11 G11:H11 H12 I13 G13 G14:I15 G16:H20 H21:H24 I16:I19 G18:G1048576 L15:O1048576 L3:L14 O4:O14 M7:M14 O3 N4:N8 N14 N10 N12">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>$B1 = "Zernike"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:D4 G1:I4 L1:R2 C5 G9:I9 G11:I11 I10 H12 I13 L3:L4 N5:R8 P3:R4 N10:R10 P9:R9 N12:R12 P11:R11 P13:R13 N14:R16 L7:M16 H14:I1048576 C18:D1048576 G20:G1048576 G18 L17:R1048576 C6:D17 G13:G17">
+  <conditionalFormatting sqref="L15:R1048576 C10:D1048576 I23:I1048576 L1:R2 C1:D9 G1:I4 G9:H9 G25:H1048576 I9:I11 G11:H11 H12 I13 G13 G14:I15 G16:H20 H21:H24 I16:I19 G18:G1048576 L3:L14 O4:R14 M7:M14 O3:R3 N4:N8 N14 N10 N12">
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>$B1 = "INIT"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D4 G1:G4 I1:K1 I9:I11 G9 G11 I3:K4 I2 I18:I1048576 I19:K1048576 D18:D1048576 G20:G1048576 G18 P18:R1048576 I16:I17 J16:K18 D6:D17 G13:G17 P1:R17 I13 J7:K13 I14:K15">
+  <conditionalFormatting sqref="D10:D1048576 P1:R1048576 D1:D9 I1:I4 G1:G4 J7:K8 J1:K1 J3:K4 G9 G11 I9:K11 I21:I1048576 J12:K1048576 I13:I19 G13:G1048576">
     <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>$B1 = "Coordinate Break"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I4 N1:R2 I9:I11 N5:R8 P3:R4 N10:R10 P9:R9 N12:R12 P11:R11 P13:R13 N18:R1048576 N14:R17 I13:I1048576">
+  <conditionalFormatting sqref="I1:I4 I9:I11 I23:I1048576 I13:I19 N1:N2 N4:N8 N10 N14:N1048576 N12 O1:R1048576">
     <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>$B1 = "Paraxial Lens"</formula>
     </cfRule>
@@ -2053,7 +2167,7 @@
       <formula>$B1 = "Slit"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:R2 N5:R8 P3:R4 N10:R10 P9:R9 N12:R12 P11:R11 P13:R13 N14:R1048576">
+  <conditionalFormatting sqref="N1:N2 N14:N1048576 N4:N8 N10 N12 O1:R1048576">
     <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>$B1 = "Obscuration"</formula>
     </cfRule>
@@ -2061,372 +2175,341 @@
       <formula>$B1 = "Standard"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
+  <conditionalFormatting sqref="G5:G8 J5:K6 I5:I8">
     <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+      <formula>$B5 = "Prism"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5:K6">
+    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+      <formula>$B5 = "Coordinate Break"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5:I8">
+    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>$B5 = "Zernike"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
-    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+  <conditionalFormatting sqref="G5:I8">
+    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>$B5 = "INIT"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
-    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
-      <formula>$B5 = "Coordinate Break"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G5:G8 I5:L6 I7:I8">
-    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
-      <formula>$B5 = "Prism"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J5:K6">
+  <conditionalFormatting sqref="G5:G8 I5:I8">
     <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>$B5 = "Coordinate Break"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5:I8 L5:L6">
+  <conditionalFormatting sqref="I5:I8">
     <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
-      <formula>$B5 = "Zernike"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G5:I8 L5:L6">
+      <formula>$B5 = "Paraxial Lens"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5:I8">
     <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
-      <formula>$B5 = "INIT"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G5:G8 I5:I8">
+      <formula>$B5 = "Slit"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:K2">
     <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
-      <formula>$B5 = "Coordinate Break"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5:I8">
+      <formula>$B2 = "Prism"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:K2">
     <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
-      <formula>$B5 = "Paraxial Lens"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5:I8">
+      <formula>$B2 = "Coordinate Break"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10">
     <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
-      <formula>$B5 = "Slit"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G10">
+      <formula>$B10 = "Prism"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10:H10">
     <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
-      <formula>$B10 = "Prism"</formula>
+      <formula>$B10 = "Zernike"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10:H10">
     <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
-      <formula>$B10 = "Zernike"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G10:H10">
+      <formula>$B10 = "INIT"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10">
     <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
-      <formula>$B10 = "INIT"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G10">
+      <formula>$B10 = "Coordinate Break"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12">
     <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
-      <formula>$B10 = "Coordinate Break"</formula>
+      <formula>$B12 = "Prism"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12">
     <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
-      <formula>$B12 = "Prism"</formula>
+      <formula>$B12 = "Zernike"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12">
     <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23">
-      <formula>$B12 = "Zernike"</formula>
+      <formula>$B12 = "INIT"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12">
     <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24">
+      <formula>$B12 = "Coordinate Break"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
+    <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25">
+      <formula>$B12 = "Prism"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
+    <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
+      <formula>$B12 = "Zernike"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
+    <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
       <formula>$B12 = "INIT"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G12">
-    <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25">
-      <formula>$B12 = "Coordinate Break"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H13">
-    <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
-      <formula>$B13 = "Zernike"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H13">
-    <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
-      <formula>$B13 = "INIT"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
     <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>$B12 = "Prism"</formula>
+      <formula>$B12 = "Coordinate Break"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
     <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29">
-      <formula>$B12 = "Zernike"</formula>
+      <formula>$B12 = "Paraxial Lens"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
     <cfRule type="expression" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30">
-      <formula>$B12 = "INIT"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
+      <formula>$B12 = "Slit"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13">
     <cfRule type="expression" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31">
-      <formula>$B12 = "Coordinate Break"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
+      <formula>$B13 = "Zernike"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13">
     <cfRule type="expression" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32">
-      <formula>$B12 = "Paraxial Lens"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
-    <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33">
-      <formula>$B12 = "Slit"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J2:K2">
-    <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
-      <formula>$B2 = "Prism"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J2:K2">
-    <cfRule type="expression" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
-      <formula>$B2 = "Coordinate Break"</formula>
+      <formula>$B13 = "INIT"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G24">
+    <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>#ref! = "Prism"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G24">
+    <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+      <formula>#ref! = "Zernike"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G24">
+    <cfRule type="expression" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>#ref! = "INIT"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G24">
+    <cfRule type="expression" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>#ref! = "Coordinate Break"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G24">
+    <cfRule type="expression" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33">
+      <formula>#ref! = "Prism"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G24">
+    <cfRule type="expression" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
+      <formula>#ref! = "Zernike"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G24">
+    <cfRule type="expression" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
+      <formula>#ref! = "INIT"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G24">
+    <cfRule type="expression" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36">
+      <formula>#ref! = "Coordinate Break"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:M6">
-    <cfRule type="expression" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36">
+    <cfRule type="expression" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37">
       <formula>$B3 = "Prism"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:M6">
-    <cfRule type="expression" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37">
+    <cfRule type="expression" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
       <formula>$B3 = "Zernike"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:M6">
-    <cfRule type="expression" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
+    <cfRule type="expression" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
       <formula>$B3 = "INIT"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:O4">
-    <cfRule type="expression" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
+  <conditionalFormatting sqref="N3">
+    <cfRule type="expression" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
       <formula>$B3 = "Prism"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:O4">
-    <cfRule type="expression" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
+  <conditionalFormatting sqref="N3">
+    <cfRule type="expression" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
       <formula>$B3 = "Zernike"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:O4">
-    <cfRule type="expression" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
+  <conditionalFormatting sqref="N3">
+    <cfRule type="expression" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
       <formula>$B3 = "INIT"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:O4">
-    <cfRule type="expression" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
+  <conditionalFormatting sqref="N3">
+    <cfRule type="expression" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43">
       <formula>$B3 = "Paraxial Lens"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:O4">
-    <cfRule type="expression" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43">
+  <conditionalFormatting sqref="N3">
+    <cfRule type="expression" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44">
       <formula>$B3 = "Standard"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:O4">
-    <cfRule type="expression" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44">
+  <conditionalFormatting sqref="N3">
+    <cfRule type="expression" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45">
       <formula>$B3 = "Slit"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N9:O9">
-    <cfRule type="expression" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45">
+  <conditionalFormatting sqref="N9">
+    <cfRule type="expression" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46">
       <formula>$B9 = "Prism"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N9:O9">
-    <cfRule type="expression" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46">
+  <conditionalFormatting sqref="N9">
+    <cfRule type="expression" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47">
       <formula>$B9 = "Zernike"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N9:O9">
-    <cfRule type="expression" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47">
+  <conditionalFormatting sqref="N9">
+    <cfRule type="expression" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
       <formula>$B9 = "INIT"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N9:O9">
-    <cfRule type="expression" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
+  <conditionalFormatting sqref="N9">
+    <cfRule type="expression" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
       <formula>$B9 = "Paraxial Lens"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N9:O9">
-    <cfRule type="expression" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
+  <conditionalFormatting sqref="N9">
+    <cfRule type="expression" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
       <formula>$B9 = "Standard"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N9:O9">
-    <cfRule type="expression" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+  <conditionalFormatting sqref="N9">
+    <cfRule type="expression" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51">
       <formula>$B9 = "Slit"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N11:O11">
-    <cfRule type="expression" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51">
+  <conditionalFormatting sqref="N11">
+    <cfRule type="expression" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52">
       <formula>$B11 = "Prism"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N11:O11">
-    <cfRule type="expression" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52">
+  <conditionalFormatting sqref="N11">
+    <cfRule type="expression" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53">
       <formula>$B11 = "Zernike"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N11:O11">
-    <cfRule type="expression" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53">
+  <conditionalFormatting sqref="N11">
+    <cfRule type="expression" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
       <formula>$B11 = "INIT"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N11:O11">
-    <cfRule type="expression" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
+  <conditionalFormatting sqref="N11">
+    <cfRule type="expression" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55">
       <formula>$B11 = "Paraxial Lens"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N11:O11">
-    <cfRule type="expression" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55">
+  <conditionalFormatting sqref="N11">
+    <cfRule type="expression" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
       <formula>$B11 = "Standard"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N11:O11">
-    <cfRule type="expression" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+  <conditionalFormatting sqref="N11">
+    <cfRule type="expression" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="57">
       <formula>$B11 = "Slit"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N13:O13">
-    <cfRule type="expression" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="57">
+  <conditionalFormatting sqref="N13">
+    <cfRule type="expression" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="58">
       <formula>$B13 = "Prism"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N13:O13">
-    <cfRule type="expression" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="58">
+  <conditionalFormatting sqref="N13">
+    <cfRule type="expression" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="59">
       <formula>$B13 = "Zernike"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N13:O13">
-    <cfRule type="expression" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="59">
+  <conditionalFormatting sqref="N13">
+    <cfRule type="expression" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="60">
       <formula>$B13 = "INIT"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N13:O13">
-    <cfRule type="expression" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="60">
+  <conditionalFormatting sqref="N13">
+    <cfRule type="expression" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="61">
       <formula>$B13 = "Paraxial Lens"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N13:O13">
-    <cfRule type="expression" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="61">
+  <conditionalFormatting sqref="N13">
+    <cfRule type="expression" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="62">
       <formula>$B13 = "Standard"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N13:O13">
-    <cfRule type="expression" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="62">
+  <conditionalFormatting sqref="N13">
+    <cfRule type="expression" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="63">
       <formula>$B13 = "Slit"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G20 I20:P20">
-    <cfRule type="expression" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
-      <formula>#ref! = "Prism"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D20 L20:O20 G20:I20 Q20:R20">
-    <cfRule type="expression" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
-      <formula>#ref! = "Zernike"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C20:D20 G20:I20 L20:R20">
-    <cfRule type="expression" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
-      <formula>#ref! = "INIT"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D20 G20 I20:K20 P20:R20">
-    <cfRule type="expression" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>#ref! = "Coordinate Break"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I20 N20:R20">
-    <cfRule type="expression" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>#ref! = "Paraxial Lens"</formula>
-    </cfRule>
-    <cfRule type="expression" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>#ref! = "Slit"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N20:R20">
-    <cfRule type="expression" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>#ref! = "Obscuration"</formula>
-    </cfRule>
-    <cfRule type="expression" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>#ref! = "Standard"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G20">
-    <cfRule type="expression" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="63">
-      <formula>#ref! = "Prism"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G20">
-    <cfRule type="expression" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
-      <formula>#ref! = "Zernike"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G20">
-    <cfRule type="expression" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
-      <formula>#ref! = "INIT"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G20">
-    <cfRule type="expression" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
-      <formula>#ref! = "Coordinate Break"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="9">
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2:B13" type="list">
-      <formula1>"INIT,Coordinate Break,Paraxial Lens,Prism,Slit,Standard,Zernike"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I2:I13" type="list">
-      <formula1>"MIRROR"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B14:B19" type="list">
-      <formula1>"INIT,Coordinate Break,Paraxial Lens,Prism,Slit,Standard,Zernike,Obscuration"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B20" type="list">
-      <formula1>"INIT,Coordinate Break,Paraxial Lens,Prism,Slit,Standard,Zernike"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" error="Please select 1 to ignore current surface, otherwise leave blank" errorTitle="Ignore current surface" operator="equal" prompt="Select 1 to ignore current surface, otherwise leave blank" promptTitle="Ignore current surface" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C14:C19" type="whole">
+    <dataValidation allowBlank="true" error="Please select 1 to ignore current surface, otherwise leave blank" errorTitle="Ignore current surface" operator="equal" prompt="Select 1 to ignore current surface, otherwise leave blank" promptTitle="Ignore current surface" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C1009" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Please select 1 to make current surface a stop, otherwise leave blank" errorTitle="Make current surface a stop" operator="equal" prompt="Select 1 to make current surface a stop, otherwise leave blank" promptTitle="Make current surface a stop" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D14:D19" type="whole">
+    <dataValidation allowBlank="true" error="Please select 1 to make current surface a stop, otherwise leave blank" errorTitle="Make current surface a stop" operator="equal" prompt="Select 1 to make current surface a stop, otherwise leave blank" promptTitle="Make current surface a stop" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D1009" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Please select 1 for saving, otherwise leave blank" errorTitle="Choose your saving option" operator="equal" prompt="Select 1 for saving, otherwise leave blank" promptTitle="Choose your saving option" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E14:E19" type="whole">
+    <dataValidation allowBlank="true" error="Please select 1 for saving, otherwise leave blank" errorTitle="Choose your saving option" operator="equal" prompt="Select 1 for saving, otherwise leave blank" promptTitle="Choose your saving option" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E25:E1009" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I16:I20" type="list">
-      <formula1>"MIRROR"</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B25:B1009" type="list">
+      <formula1>"INIT,Coordinate Break,Obscuration,Paraxial Lens,Prism,Slit,Standard,Zernike"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I14:I15" type="list">
-      <formula1>"MIRROR"</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I2:I4 I9:I11 I13 I15 I23:I1009" type="list">
+      <formula1>"SPACE,MIRROR,BK7,SAPPHIRE,SF11,CAF2,ZNSE,BAF2"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2:B24" type="list">
+      <formula1>"INIT,Coordinate Break,Obscuration,Paraxial Lens,Prism,Slit,Standard,Zernike"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" error="Please select 1 for saving, otherwise leave blank" errorTitle="Choose your saving option" operator="equal" prompt="Select 1 for saving, otherwise leave blank" promptTitle="Choose your saving option" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E14:E17" type="whole">
+      <formula1>1</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" error="Please select 1 for saving, otherwise leave blank" errorTitle="Choose your saving option" operator="equal" prompt="Select 1 for saving, otherwise leave blank" promptTitle="Choose your saving option" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E18:E23" type="whole">
+      <formula1>1</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I5:I8 I12 I14 I16:I22" type="list">
+      <formula1>"SPACE,MIRROR,BK7,SAPPHIRE,SF11,CAF2,ZNSE,BAF2"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -2447,45 +2530,45 @@
   </sheetPr>
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="12" t="n">
+        <v>56</v>
+      </c>
+      <c r="B1" s="14" t="n">
         <v>3E-006</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="14" t="n">
+        <v>59</v>
+      </c>
+      <c r="B3" s="16" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="17" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2493,7 +2576,7 @@
       <c r="A5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="B5" s="16" t="n">
+      <c r="B5" s="18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2501,7 +2584,7 @@
       <c r="A6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B6" s="16" t="n">
+      <c r="B6" s="18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2509,7 +2592,7 @@
       <c r="A7" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B7" s="16" t="n">
+      <c r="B7" s="18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2517,7 +2600,7 @@
       <c r="A8" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B8" s="16" t="n">
+      <c r="B8" s="18" t="n">
         <v>5.0917</v>
       </c>
     </row>
@@ -2525,7 +2608,7 @@
       <c r="A9" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B9" s="16" t="n">
+      <c r="B9" s="18" t="n">
         <v>-1.4367</v>
       </c>
     </row>
@@ -2533,7 +2616,7 @@
       <c r="A10" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B10" s="16" t="n">
+      <c r="B10" s="18" t="n">
         <v>0.0439</v>
       </c>
     </row>
@@ -2541,7 +2624,7 @@
       <c r="A11" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B11" s="16" t="n">
+      <c r="B11" s="18" t="n">
         <v>0.0003</v>
       </c>
     </row>
@@ -2549,7 +2632,7 @@
       <c r="A12" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B12" s="16" t="n">
+      <c r="B12" s="18" t="n">
         <v>-0.0168</v>
       </c>
     </row>
@@ -2557,7 +2640,7 @@
       <c r="A13" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B13" s="16" t="n">
+      <c r="B13" s="18" t="n">
         <v>0.284</v>
       </c>
     </row>
@@ -2565,7 +2648,7 @@
       <c r="A14" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="B14" s="16" t="n">
+      <c r="B14" s="18" t="n">
         <v>0.6854</v>
       </c>
     </row>
@@ -2573,7 +2656,7 @@
       <c r="A15" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B15" s="16" t="n">
+      <c r="B15" s="18" t="n">
         <v>-0.334</v>
       </c>
     </row>
@@ -2581,7 +2664,7 @@
       <c r="A16" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="B16" s="16" t="n">
+      <c r="B16" s="18" t="n">
         <v>0.3551</v>
       </c>
     </row>
@@ -2589,7 +2672,7 @@
       <c r="A17" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="B17" s="16" t="n">
+      <c r="B17" s="18" t="n">
         <v>-0.2928</v>
       </c>
     </row>
@@ -2597,7 +2680,7 @@
       <c r="A18" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="B18" s="16" t="n">
+      <c r="B18" s="18" t="n">
         <v>-0.0011</v>
       </c>
     </row>
@@ -2605,7 +2688,7 @@
       <c r="A19" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B19" s="16" t="n">
+      <c r="B19" s="18" t="n">
         <v>-0.0012</v>
       </c>
     </row>
@@ -2613,7 +2696,7 @@
       <c r="A20" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B20" s="16" t="n">
+      <c r="B20" s="18" t="n">
         <v>0.0007</v>
       </c>
     </row>
@@ -2621,7 +2704,7 @@
       <c r="A21" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="B21" s="16" t="n">
+      <c r="B21" s="18" t="n">
         <v>0.0022</v>
       </c>
     </row>
@@ -2629,7 +2712,7 @@
       <c r="A22" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="B22" s="16" t="n">
+      <c r="B22" s="18" t="n">
         <v>-0.0012</v>
       </c>
     </row>
@@ -2637,7 +2720,7 @@
       <c r="A23" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="B23" s="16" t="n">
+      <c r="B23" s="18" t="n">
         <v>-0.0108</v>
       </c>
     </row>
@@ -2645,7 +2728,7 @@
       <c r="A24" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="B24" s="16" t="n">
+      <c r="B24" s="18" t="n">
         <v>-0.0164</v>
       </c>
     </row>
@@ -2653,7 +2736,7 @@
       <c r="A25" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B25" s="16" t="n">
+      <c r="B25" s="18" t="n">
         <v>-0.1403</v>
       </c>
     </row>
@@ -2661,7 +2744,7 @@
       <c r="A26" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B26" s="16" t="n">
+      <c r="B26" s="18" t="n">
         <v>0.1089</v>
       </c>
     </row>
@@ -2669,7 +2752,7 @@
       <c r="A27" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="B27" s="16" t="n">
+      <c r="B27" s="18" t="n">
         <v>-0.1762</v>
       </c>
     </row>
@@ -2677,7 +2760,7 @@
       <c r="A28" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="B28" s="16" t="n">
+      <c r="B28" s="18" t="n">
         <v>0.3467</v>
       </c>
     </row>
@@ -2685,7 +2768,7 @@
       <c r="A29" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B29" s="16" t="n">
+      <c r="B29" s="18" t="n">
         <v>-0.1763</v>
       </c>
     </row>
@@ -2693,7 +2776,7 @@
       <c r="A30" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B30" s="16" t="n">
+      <c r="B30" s="18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2701,7 +2784,7 @@
       <c r="A31" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="B31" s="16" t="n">
+      <c r="B31" s="18" t="n">
         <v>-0.0002</v>
       </c>
     </row>
@@ -2709,7 +2792,7 @@
       <c r="A32" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="B32" s="16" t="n">
+      <c r="B32" s="18" t="n">
         <v>0.0007</v>
       </c>
     </row>
@@ -2717,7 +2800,7 @@
       <c r="A33" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="B33" s="16" t="n">
+      <c r="B33" s="18" t="n">
         <v>-0.0007</v>
       </c>
     </row>
@@ -2725,7 +2808,7 @@
       <c r="A34" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="B34" s="16" t="n">
+      <c r="B34" s="18" t="n">
         <v>-0.0002</v>
       </c>
     </row>
@@ -2733,7 +2816,7 @@
       <c r="A35" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B35" s="16" t="n">
+      <c r="B35" s="18" t="n">
         <v>0.0009</v>
       </c>
     </row>
@@ -2741,7 +2824,7 @@
       <c r="A36" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B36" s="16" t="n">
+      <c r="B36" s="18" t="n">
         <v>-0.0004</v>
       </c>
     </row>
@@ -2749,7 +2832,7 @@
       <c r="A37" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B37" s="16" t="n">
+      <c r="B37" s="18" t="n">
         <v>-0.0527</v>
       </c>
     </row>
@@ -2757,7 +2840,7 @@
       <c r="A38" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="B38" s="16" t="n">
+      <c r="B38" s="18" t="n">
         <v>0.0166</v>
       </c>
     </row>
@@ -2765,7 +2848,7 @@
       <c r="A39" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="B39" s="16" t="n">
+      <c r="B39" s="18" t="n">
         <v>-0.0143</v>
       </c>
     </row>
@@ -2773,12 +2856,12 @@
       <c r="A40" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="B40" s="16" t="n">
+      <c r="B40" s="18" t="n">
         <v>0.056</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="12"/>
+      <c r="B42" s="14"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -2792,11 +2875,11 @@
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>